<commit_message>
with improved excel docu
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga46yeg\Downloads\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga46yeg\GitHub\op_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAEF5A2-1A67-4560-A060-FA978432DCB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7830880D-4731-43D2-AD49-B28901E4BC09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" activeTab="3" xr2:uid="{D5A23CC1-6C90-B740-9D50-F88189E84897}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="OS2" sheetId="9" r:id="rId2"/>
     <sheet name="OS3" sheetId="10" r:id="rId3"/>
     <sheet name="OS4" sheetId="1" r:id="rId4"/>
-    <sheet name="Tabelle2" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="Tabelle1" sheetId="11" state="hidden" r:id="rId5"/>
+    <sheet name="Tabelle2" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="84">
   <si>
     <t>Pat. Nummer</t>
   </si>
@@ -787,9 +788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F264F92-B095-CB4A-93C1-0DB25CFF6E6D}">
   <dimension ref="A1:AQ109"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W111" sqref="W111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10109,7 +10110,7 @@
         <v>86</v>
       </c>
       <c r="G86">
-        <v>895</v>
+        <v>89.5</v>
       </c>
       <c r="H86">
         <v>82</v>
@@ -12013,7 +12014,7 @@
         <v>84</v>
       </c>
       <c r="G102">
-        <v>895</v>
+        <v>89.5</v>
       </c>
       <c r="H102">
         <v>84.6</v>
@@ -12958,8 +12959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF04AFBE-6FDC-204A-931F-9DA79BDC544F}">
   <dimension ref="A1:BP109"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A34" zoomScale="92" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25187,7 +25188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6021874-68DA-5A48-B581-0EC306AB7B48}">
   <dimension ref="A1:AQ109"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -37353,10 +37354,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B857DF-CD31-3C4F-B05D-3FAF23727795}">
   <dimension ref="A1:AT133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A32" sqref="A32"/>
-      <selection pane="topRight" activeCell="S20" sqref="S20"/>
+      <selection pane="topRight" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40943,34 +40944,37 @@
         <v>10</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L58" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H58" s="2" t="s">
+      <c r="M58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N58" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="O58" s="4" t="s">
         <v>26</v>
@@ -41079,7 +41083,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -41127,7 +41131,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -41166,35 +41170,35 @@
       <c r="C61" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61">
+        <v>700.9</v>
+      </c>
+      <c r="E61">
+        <v>-18</v>
+      </c>
+      <c r="F61">
+        <v>73</v>
+      </c>
+      <c r="G61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H61">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I61" t="s">
+        <v>41</v>
+      </c>
+      <c r="J61" t="s">
+        <v>38</v>
+      </c>
+      <c r="K61" t="s">
+        <v>42</v>
+      </c>
+      <c r="L61" t="s">
         <v>39</v>
       </c>
-      <c r="E61" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" t="s">
-        <v>41</v>
-      </c>
-      <c r="G61" t="s">
-        <v>42</v>
-      </c>
-      <c r="H61">
+      <c r="N61">
         <v>77.599999999999994</v>
-      </c>
-      <c r="I61">
-        <v>700.9</v>
-      </c>
-      <c r="J61">
-        <v>-18</v>
-      </c>
-      <c r="K61">
-        <v>73</v>
-      </c>
-      <c r="L61">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="M61" t="s">
-        <v>38</v>
       </c>
       <c r="P61">
         <v>704</v>
@@ -41293,32 +41297,33 @@
       <c r="C63" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="17">
+        <v>864</v>
+      </c>
+      <c r="E63" s="17">
+        <v>-17</v>
+      </c>
+      <c r="G63" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H63" s="17">
+        <v>6.2</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J63" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K63" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L63" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E63" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F63" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G63" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="H63" s="17">
+      <c r="M63"/>
+      <c r="N63" s="17">
         <v>82.1</v>
-      </c>
-      <c r="I63" s="17">
-        <v>864</v>
-      </c>
-      <c r="J63" s="17">
-        <v>-17</v>
-      </c>
-      <c r="L63" s="17">
-        <v>6.2</v>
-      </c>
-      <c r="M63" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="R63" s="17">
         <v>49.9</v>
@@ -41337,32 +41342,32 @@
       <c r="C64" t="s">
         <v>37</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64">
+        <v>793.2</v>
+      </c>
+      <c r="E64">
+        <v>-13</v>
+      </c>
+      <c r="G64" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64">
+        <v>5.4</v>
+      </c>
+      <c r="I64" t="s">
+        <v>51</v>
+      </c>
+      <c r="J64" t="s">
+        <v>48</v>
+      </c>
+      <c r="K64" t="s">
+        <v>52</v>
+      </c>
+      <c r="L64" t="s">
         <v>49</v>
       </c>
-      <c r="E64" t="s">
-        <v>50</v>
-      </c>
-      <c r="F64" t="s">
-        <v>51</v>
-      </c>
-      <c r="G64" t="s">
-        <v>52</v>
-      </c>
-      <c r="H64">
+      <c r="N64">
         <v>88.2</v>
-      </c>
-      <c r="I64">
-        <v>793.2</v>
-      </c>
-      <c r="J64">
-        <v>-13</v>
-      </c>
-      <c r="L64">
-        <v>5.4</v>
-      </c>
-      <c r="M64" t="s">
-        <v>48</v>
       </c>
       <c r="P64">
         <v>796</v>
@@ -41453,32 +41458,32 @@
       <c r="C65" t="s">
         <v>36</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65">
+        <v>852</v>
+      </c>
+      <c r="E65">
+        <v>-16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65">
+        <v>7.3</v>
+      </c>
+      <c r="I65" t="s">
+        <v>56</v>
+      </c>
+      <c r="J65" t="s">
+        <v>53</v>
+      </c>
+      <c r="K65" t="s">
+        <v>57</v>
+      </c>
+      <c r="L65" t="s">
         <v>54</v>
       </c>
-      <c r="E65" t="s">
-        <v>55</v>
-      </c>
-      <c r="F65" t="s">
-        <v>56</v>
-      </c>
-      <c r="G65" t="s">
-        <v>57</v>
-      </c>
-      <c r="H65">
+      <c r="N65">
         <v>88.9</v>
-      </c>
-      <c r="I65">
-        <v>852</v>
-      </c>
-      <c r="J65">
-        <v>-16</v>
-      </c>
-      <c r="L65">
-        <v>7.3</v>
-      </c>
-      <c r="M65" t="s">
-        <v>53</v>
       </c>
       <c r="P65">
         <v>852</v>
@@ -41570,31 +41575,31 @@
         <v>36</v>
       </c>
       <c r="D66">
+        <v>771.3</v>
+      </c>
+      <c r="E66">
+        <v>-43.4</v>
+      </c>
+      <c r="G66">
+        <v>85.7</v>
+      </c>
+      <c r="H66">
+        <v>3.5</v>
+      </c>
+      <c r="I66">
+        <v>84.8</v>
+      </c>
+      <c r="J66">
+        <v>-2.6</v>
+      </c>
+      <c r="K66">
+        <v>95.3</v>
+      </c>
+      <c r="L66">
         <v>13.1</v>
       </c>
-      <c r="E66">
-        <v>85.7</v>
-      </c>
-      <c r="F66">
-        <v>84.8</v>
-      </c>
-      <c r="G66">
-        <v>95.3</v>
-      </c>
-      <c r="H66">
+      <c r="N66">
         <v>88.1</v>
-      </c>
-      <c r="I66">
-        <v>771.3</v>
-      </c>
-      <c r="J66">
-        <v>-43.4</v>
-      </c>
-      <c r="L66">
-        <v>3.5</v>
-      </c>
-      <c r="M66">
-        <v>-2.6</v>
       </c>
       <c r="P66">
         <v>783</v>
@@ -41685,32 +41690,32 @@
       <c r="C67" t="s">
         <v>36</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67">
+        <v>882.2</v>
+      </c>
+      <c r="E67">
+        <v>-21.5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>60</v>
+      </c>
+      <c r="H67">
+        <v>6.5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>61</v>
+      </c>
+      <c r="J67" t="s">
+        <v>58</v>
+      </c>
+      <c r="K67" t="s">
+        <v>62</v>
+      </c>
+      <c r="L67" t="s">
         <v>59</v>
       </c>
-      <c r="E67" t="s">
-        <v>60</v>
-      </c>
-      <c r="F67" t="s">
-        <v>61</v>
-      </c>
-      <c r="G67" t="s">
-        <v>62</v>
-      </c>
-      <c r="H67">
+      <c r="N67">
         <v>84.6</v>
-      </c>
-      <c r="I67">
-        <v>882.2</v>
-      </c>
-      <c r="J67">
-        <v>-21.5</v>
-      </c>
-      <c r="L67">
-        <v>6.5</v>
-      </c>
-      <c r="M67" t="s">
-        <v>58</v>
       </c>
       <c r="P67">
         <v>886</v>
@@ -41809,32 +41814,32 @@
       <c r="C69" t="s">
         <v>36</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69">
+        <v>683.3</v>
+      </c>
+      <c r="E69">
+        <v>-39.4</v>
+      </c>
+      <c r="G69" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I69" t="s">
+        <v>65</v>
+      </c>
+      <c r="J69">
+        <v>0.1</v>
+      </c>
+      <c r="K69" t="s">
+        <v>66</v>
+      </c>
+      <c r="L69" t="s">
         <v>63</v>
       </c>
-      <c r="E69" t="s">
-        <v>64</v>
-      </c>
-      <c r="F69" t="s">
-        <v>65</v>
-      </c>
-      <c r="G69" t="s">
-        <v>66</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="N69" t="s">
         <v>67</v>
-      </c>
-      <c r="I69">
-        <v>683.3</v>
-      </c>
-      <c r="J69">
-        <v>-39.4</v>
-      </c>
-      <c r="L69">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M69">
-        <v>0.1</v>
       </c>
       <c r="P69">
         <v>697</v>
@@ -41925,32 +41930,32 @@
       <c r="C70" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70">
+        <v>800</v>
+      </c>
+      <c r="E70">
+        <v>-31</v>
+      </c>
+      <c r="G70" s="6">
+        <v>97.6</v>
+      </c>
+      <c r="H70">
+        <v>7.8</v>
+      </c>
+      <c r="I70" s="6">
+        <v>85.4</v>
+      </c>
+      <c r="J70">
+        <v>9.6</v>
+      </c>
+      <c r="K70" s="6">
+        <v>84.6</v>
+      </c>
+      <c r="L70" s="6">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E70" s="6">
-        <v>97.6</v>
-      </c>
-      <c r="F70" s="6">
-        <v>85.4</v>
-      </c>
-      <c r="G70" s="6">
-        <v>84.6</v>
-      </c>
-      <c r="H70" s="6">
+      <c r="N70" s="6">
         <v>84.9</v>
-      </c>
-      <c r="I70">
-        <v>800</v>
-      </c>
-      <c r="J70">
-        <v>-31</v>
-      </c>
-      <c r="L70">
-        <v>7.8</v>
-      </c>
-      <c r="M70">
-        <v>9.6</v>
       </c>
       <c r="P70">
         <v>806</v>
@@ -41987,32 +41992,32 @@
       <c r="C71" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71">
+        <v>802</v>
+      </c>
+      <c r="E71">
+        <v>-19</v>
+      </c>
+      <c r="G71" s="6">
+        <v>96.2</v>
+      </c>
+      <c r="H71">
+        <v>5</v>
+      </c>
+      <c r="I71" s="6">
+        <v>87</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71" s="6">
+        <v>92.5</v>
+      </c>
+      <c r="L71" s="6">
         <v>5.5</v>
       </c>
-      <c r="E71" s="6">
-        <v>96.2</v>
-      </c>
-      <c r="F71" s="6">
-        <v>87</v>
-      </c>
-      <c r="G71" s="6">
-        <v>92.5</v>
-      </c>
-      <c r="H71" s="6">
+      <c r="N71" s="6">
         <v>84.4</v>
-      </c>
-      <c r="I71">
-        <v>802</v>
-      </c>
-      <c r="J71">
-        <v>-19</v>
-      </c>
-      <c r="L71">
-        <v>5</v>
-      </c>
-      <c r="M71">
-        <v>0</v>
       </c>
       <c r="P71">
         <v>806</v>
@@ -42049,32 +42054,32 @@
       <c r="C72" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72">
+        <v>867</v>
+      </c>
+      <c r="E72">
+        <v>-20</v>
+      </c>
+      <c r="G72" s="6">
+        <v>96.9</v>
+      </c>
+      <c r="H72">
+        <v>6.2</v>
+      </c>
+      <c r="I72" s="6">
+        <v>85.5</v>
+      </c>
+      <c r="J72">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="K72" s="6">
+        <v>88.7</v>
+      </c>
+      <c r="L72" s="6">
         <v>5.4</v>
       </c>
-      <c r="E72" s="6">
-        <v>96.9</v>
-      </c>
-      <c r="F72" s="6">
-        <v>85.5</v>
-      </c>
-      <c r="G72" s="6">
-        <v>88.7</v>
-      </c>
-      <c r="H72" s="6">
+      <c r="N72" s="6">
         <v>82.9</v>
-      </c>
-      <c r="I72">
-        <v>867</v>
-      </c>
-      <c r="J72">
-        <v>-20</v>
-      </c>
-      <c r="L72">
-        <v>6.2</v>
-      </c>
-      <c r="M72">
-        <v>-2.2000000000000002</v>
       </c>
       <c r="P72">
         <v>871</v>
@@ -42111,32 +42116,32 @@
       <c r="C73" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73">
+        <v>817</v>
+      </c>
+      <c r="E73">
+        <v>-9</v>
+      </c>
+      <c r="G73" s="6">
+        <v>84.2</v>
+      </c>
+      <c r="H73">
+        <v>6.5</v>
+      </c>
+      <c r="I73" s="6">
+        <v>84.7</v>
+      </c>
+      <c r="J73">
+        <v>-0.7</v>
+      </c>
+      <c r="K73" s="6">
+        <v>86.6</v>
+      </c>
+      <c r="L73" s="6">
         <v>2.5</v>
       </c>
-      <c r="E73" s="6">
-        <v>84.2</v>
-      </c>
-      <c r="F73" s="6">
-        <v>84.7</v>
-      </c>
-      <c r="G73" s="6">
-        <v>86.6</v>
-      </c>
-      <c r="H73" s="6">
+      <c r="N73" s="6">
         <v>81.3</v>
-      </c>
-      <c r="I73">
-        <v>817</v>
-      </c>
-      <c r="J73">
-        <v>-9</v>
-      </c>
-      <c r="L73">
-        <v>6.5</v>
-      </c>
-      <c r="M73">
-        <v>-0.7</v>
       </c>
       <c r="P73">
         <v>818</v>
@@ -42174,31 +42179,31 @@
         <v>37</v>
       </c>
       <c r="D74">
+        <v>806</v>
+      </c>
+      <c r="E74">
+        <v>-24</v>
+      </c>
+      <c r="G74">
+        <v>92.1</v>
+      </c>
+      <c r="H74">
+        <v>4.8</v>
+      </c>
+      <c r="I74">
+        <v>83.6</v>
+      </c>
+      <c r="J74">
+        <v>0.7</v>
+      </c>
+      <c r="K74">
+        <v>91.1</v>
+      </c>
+      <c r="L74">
         <v>6.9</v>
       </c>
-      <c r="E74">
-        <v>92.1</v>
-      </c>
-      <c r="F74">
-        <v>83.6</v>
-      </c>
-      <c r="G74">
-        <v>91.1</v>
-      </c>
-      <c r="H74">
+      <c r="N74">
         <v>84.7</v>
-      </c>
-      <c r="I74">
-        <v>806</v>
-      </c>
-      <c r="J74">
-        <v>-24</v>
-      </c>
-      <c r="L74">
-        <v>4.8</v>
-      </c>
-      <c r="M74">
-        <v>0.7</v>
       </c>
       <c r="P74">
         <v>812</v>
@@ -42236,31 +42241,31 @@
         <v>36</v>
       </c>
       <c r="D75">
+        <v>748</v>
+      </c>
+      <c r="E75">
+        <v>-27</v>
+      </c>
+      <c r="G75">
+        <v>92.9</v>
+      </c>
+      <c r="H75">
+        <v>5.2</v>
+      </c>
+      <c r="I75">
+        <v>84.3</v>
+      </c>
+      <c r="J75">
+        <v>-3.5</v>
+      </c>
+      <c r="K75">
+        <v>89</v>
+      </c>
+      <c r="L75">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E75">
-        <v>92.9</v>
-      </c>
-      <c r="F75">
-        <v>84.3</v>
-      </c>
-      <c r="G75">
-        <v>89</v>
-      </c>
-      <c r="H75">
+      <c r="N75">
         <v>87</v>
-      </c>
-      <c r="I75">
-        <v>748</v>
-      </c>
-      <c r="J75">
-        <v>-27</v>
-      </c>
-      <c r="L75">
-        <v>5.2</v>
-      </c>
-      <c r="M75">
-        <v>-3.5</v>
       </c>
       <c r="P75">
         <v>754</v>
@@ -42298,31 +42303,31 @@
         <v>37</v>
       </c>
       <c r="D76">
+        <v>896</v>
+      </c>
+      <c r="E76">
+        <v>-14</v>
+      </c>
+      <c r="G76">
+        <v>86.9</v>
+      </c>
+      <c r="H76">
+        <v>6.4</v>
+      </c>
+      <c r="I76">
+        <v>85.7</v>
+      </c>
+      <c r="J76">
+        <v>-0.7</v>
+      </c>
+      <c r="K76">
+        <v>88.6</v>
+      </c>
+      <c r="L76">
         <v>3.5</v>
       </c>
-      <c r="E76">
-        <v>86.9</v>
-      </c>
-      <c r="F76">
-        <v>85.7</v>
-      </c>
-      <c r="G76">
-        <v>88.6</v>
-      </c>
-      <c r="H76">
+      <c r="N76">
         <v>86.7</v>
-      </c>
-      <c r="I76">
-        <v>896</v>
-      </c>
-      <c r="J76">
-        <v>-14</v>
-      </c>
-      <c r="L76">
-        <v>6.4</v>
-      </c>
-      <c r="M76">
-        <v>-0.7</v>
       </c>
       <c r="P76">
         <v>899</v>
@@ -42360,31 +42365,32 @@
         <v>36</v>
       </c>
       <c r="D77" s="10">
+        <v>799</v>
+      </c>
+      <c r="E77" s="10">
+        <v>-10</v>
+      </c>
+      <c r="G77" s="10">
+        <v>98</v>
+      </c>
+      <c r="H77" s="10">
+        <v>6.3</v>
+      </c>
+      <c r="I77" s="10">
+        <v>85.9</v>
+      </c>
+      <c r="J77" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="K77" s="10">
+        <v>89.1</v>
+      </c>
+      <c r="L77" s="10">
         <v>3</v>
       </c>
-      <c r="E77" s="10">
-        <v>98</v>
-      </c>
-      <c r="F77" s="10">
-        <v>85.9</v>
-      </c>
-      <c r="G77" s="10">
-        <v>89.1</v>
-      </c>
-      <c r="H77" s="10">
+      <c r="M77"/>
+      <c r="N77" s="10">
         <v>90.5</v>
-      </c>
-      <c r="I77" s="10">
-        <v>799</v>
-      </c>
-      <c r="J77" s="10">
-        <v>-10</v>
-      </c>
-      <c r="L77" s="10">
-        <v>6.3</v>
-      </c>
-      <c r="M77" s="10">
-        <v>0.2</v>
       </c>
       <c r="P77" s="10">
         <v>801</v>
@@ -42422,31 +42428,31 @@
         <v>36</v>
       </c>
       <c r="D78">
+        <v>836</v>
+      </c>
+      <c r="E78">
+        <v>-13</v>
+      </c>
+      <c r="G78">
+        <v>87.5</v>
+      </c>
+      <c r="H78">
+        <v>6.3</v>
+      </c>
+      <c r="I78">
+        <v>87.5</v>
+      </c>
+      <c r="J78">
+        <v>0.7</v>
+      </c>
+      <c r="K78">
+        <v>91.6</v>
+      </c>
+      <c r="L78">
         <v>3.4</v>
       </c>
-      <c r="E78">
-        <v>87.5</v>
-      </c>
-      <c r="F78">
-        <v>87.5</v>
-      </c>
-      <c r="G78">
-        <v>91.6</v>
-      </c>
-      <c r="H78">
+      <c r="N78">
         <v>90.8</v>
-      </c>
-      <c r="I78">
-        <v>836</v>
-      </c>
-      <c r="J78">
-        <v>-13</v>
-      </c>
-      <c r="L78">
-        <v>6.3</v>
-      </c>
-      <c r="M78">
-        <v>0.7</v>
       </c>
       <c r="P78">
         <v>838</v>
@@ -42484,31 +42490,31 @@
         <v>36</v>
       </c>
       <c r="D79">
+        <v>830</v>
+      </c>
+      <c r="E79">
+        <v>-14</v>
+      </c>
+      <c r="G79">
+        <v>89.2</v>
+      </c>
+      <c r="H79">
+        <v>6.7</v>
+      </c>
+      <c r="I79">
+        <v>89</v>
+      </c>
+      <c r="J79">
+        <v>-1.7</v>
+      </c>
+      <c r="K79">
+        <v>91.1</v>
+      </c>
+      <c r="L79">
         <v>3.8</v>
       </c>
-      <c r="E79">
-        <v>89.2</v>
-      </c>
-      <c r="F79">
-        <v>89</v>
-      </c>
-      <c r="G79">
-        <v>91.1</v>
-      </c>
-      <c r="H79">
+      <c r="N79">
         <v>89.6</v>
-      </c>
-      <c r="I79">
-        <v>830</v>
-      </c>
-      <c r="J79">
-        <v>-14</v>
-      </c>
-      <c r="L79">
-        <v>6.7</v>
-      </c>
-      <c r="M79">
-        <v>-1.7</v>
       </c>
       <c r="P79">
         <v>832</v>
@@ -42546,31 +42552,31 @@
         <v>36</v>
       </c>
       <c r="D80">
+        <v>814</v>
+      </c>
+      <c r="E80">
+        <v>-9</v>
+      </c>
+      <c r="G80">
+        <v>75.5</v>
+      </c>
+      <c r="H80">
+        <v>5</v>
+      </c>
+      <c r="I80">
+        <v>85.5</v>
+      </c>
+      <c r="J80">
+        <v>-0.2</v>
+      </c>
+      <c r="K80">
+        <v>87.9</v>
+      </c>
+      <c r="L80">
         <v>2.6</v>
       </c>
-      <c r="E80">
-        <v>75.5</v>
-      </c>
-      <c r="F80">
-        <v>85.5</v>
-      </c>
-      <c r="G80">
-        <v>87.9</v>
-      </c>
-      <c r="H80">
+      <c r="N80">
         <v>79.5</v>
-      </c>
-      <c r="I80">
-        <v>814</v>
-      </c>
-      <c r="J80">
-        <v>-9</v>
-      </c>
-      <c r="L80">
-        <v>5</v>
-      </c>
-      <c r="M80">
-        <v>-0.2</v>
       </c>
       <c r="P80">
         <v>815</v>
@@ -42608,31 +42614,32 @@
         <v>37</v>
       </c>
       <c r="D81" s="10">
+        <v>935</v>
+      </c>
+      <c r="E81" s="10">
+        <v>-11</v>
+      </c>
+      <c r="G81" s="10">
+        <v>88.8</v>
+      </c>
+      <c r="H81" s="10">
+        <v>7.3</v>
+      </c>
+      <c r="I81" s="10">
+        <v>90.6</v>
+      </c>
+      <c r="J81" s="10">
+        <v>-2.7</v>
+      </c>
+      <c r="K81" s="10">
+        <v>90.5</v>
+      </c>
+      <c r="L81" s="10">
         <v>2.5</v>
       </c>
-      <c r="E81" s="10">
-        <v>88.8</v>
-      </c>
-      <c r="F81" s="10">
-        <v>90.6</v>
-      </c>
-      <c r="G81" s="10">
-        <v>90.5</v>
-      </c>
-      <c r="H81" s="10">
+      <c r="M81"/>
+      <c r="N81" s="10">
         <v>78.2</v>
-      </c>
-      <c r="I81" s="10">
-        <v>935</v>
-      </c>
-      <c r="J81" s="10">
-        <v>-11</v>
-      </c>
-      <c r="L81" s="10">
-        <v>7.3</v>
-      </c>
-      <c r="M81" s="10">
-        <v>-2.7</v>
       </c>
       <c r="P81" s="10">
         <v>936</v>
@@ -42670,31 +42677,32 @@
         <v>36</v>
       </c>
       <c r="D82" s="10">
+        <v>818</v>
+      </c>
+      <c r="E82" s="10">
+        <v>-10</v>
+      </c>
+      <c r="G82" s="10">
+        <v>92</v>
+      </c>
+      <c r="H82" s="10">
+        <v>7.8</v>
+      </c>
+      <c r="I82" s="10">
+        <v>88.4</v>
+      </c>
+      <c r="J82" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="K82" s="10">
+        <v>92.6</v>
+      </c>
+      <c r="L82" s="10">
         <v>2.9</v>
       </c>
-      <c r="E82" s="10">
-        <v>92</v>
-      </c>
-      <c r="F82" s="10">
-        <v>88.4</v>
-      </c>
-      <c r="G82" s="10">
-        <v>92.6</v>
-      </c>
-      <c r="H82" s="10">
+      <c r="M82"/>
+      <c r="N82" s="10">
         <v>87.1</v>
-      </c>
-      <c r="I82" s="10">
-        <v>818</v>
-      </c>
-      <c r="J82" s="10">
-        <v>-10</v>
-      </c>
-      <c r="L82" s="10">
-        <v>7.8</v>
-      </c>
-      <c r="M82" s="10">
-        <v>1.4</v>
       </c>
       <c r="P82" s="10">
         <v>819</v>
@@ -42732,31 +42740,32 @@
         <v>36</v>
       </c>
       <c r="D83" s="10">
+        <v>803</v>
+      </c>
+      <c r="E83" s="10">
+        <v>-5</v>
+      </c>
+      <c r="G83" s="10">
+        <v>90.1</v>
+      </c>
+      <c r="H83" s="10">
+        <v>5.7</v>
+      </c>
+      <c r="I83" s="10">
+        <v>84.1</v>
+      </c>
+      <c r="J83" s="10">
+        <v>-1.7</v>
+      </c>
+      <c r="K83" s="10">
+        <v>83.7</v>
+      </c>
+      <c r="L83" s="10">
         <v>1.3</v>
       </c>
-      <c r="E83" s="10">
-        <v>90.1</v>
-      </c>
-      <c r="F83" s="10">
-        <v>84.1</v>
-      </c>
-      <c r="G83" s="10">
-        <v>83.7</v>
-      </c>
-      <c r="H83" s="10">
+      <c r="M83"/>
+      <c r="N83" s="10">
         <v>88</v>
-      </c>
-      <c r="I83" s="10">
-        <v>803</v>
-      </c>
-      <c r="J83" s="10">
-        <v>-5</v>
-      </c>
-      <c r="L83" s="10">
-        <v>5.7</v>
-      </c>
-      <c r="M83" s="10">
-        <v>-1.7</v>
       </c>
       <c r="P83" s="10">
         <v>804</v>
@@ -42794,31 +42803,31 @@
         <v>36</v>
       </c>
       <c r="D84">
+        <v>781</v>
+      </c>
+      <c r="E84">
+        <v>-11</v>
+      </c>
+      <c r="G84">
+        <v>94.3</v>
+      </c>
+      <c r="H84">
+        <v>6.4</v>
+      </c>
+      <c r="I84">
+        <v>84</v>
+      </c>
+      <c r="J84">
+        <v>-1.3</v>
+      </c>
+      <c r="K84">
+        <v>86</v>
+      </c>
+      <c r="L84">
         <v>3.3</v>
       </c>
-      <c r="E84">
-        <v>94.3</v>
-      </c>
-      <c r="F84">
-        <v>84</v>
-      </c>
-      <c r="G84">
-        <v>86</v>
-      </c>
-      <c r="H84">
+      <c r="N84">
         <v>85.5</v>
-      </c>
-      <c r="I84">
-        <v>781</v>
-      </c>
-      <c r="J84">
-        <v>-11</v>
-      </c>
-      <c r="L84">
-        <v>6.4</v>
-      </c>
-      <c r="M84">
-        <v>-1.3</v>
       </c>
       <c r="P84">
         <v>783</v>
@@ -42856,31 +42865,31 @@
         <v>36</v>
       </c>
       <c r="D85">
+        <v>881</v>
+      </c>
+      <c r="E85">
+        <v>-33</v>
+      </c>
+      <c r="G85">
+        <v>99.9</v>
+      </c>
+      <c r="H85">
+        <v>5.6</v>
+      </c>
+      <c r="I85">
+        <v>86.4</v>
+      </c>
+      <c r="J85">
+        <v>-3.8</v>
+      </c>
+      <c r="K85">
+        <v>91.2</v>
+      </c>
+      <c r="L85">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E85">
-        <v>99.9</v>
-      </c>
-      <c r="F85">
-        <v>86.4</v>
-      </c>
-      <c r="G85">
-        <v>91.2</v>
-      </c>
-      <c r="H85">
+      <c r="N85">
         <v>75.900000000000006</v>
-      </c>
-      <c r="I85">
-        <v>881</v>
-      </c>
-      <c r="J85">
-        <v>-33</v>
-      </c>
-      <c r="L85">
-        <v>5.6</v>
-      </c>
-      <c r="M85">
-        <v>-3.8</v>
       </c>
       <c r="P85">
         <v>889</v>
@@ -42918,31 +42927,31 @@
         <v>37</v>
       </c>
       <c r="D86">
+        <v>854</v>
+      </c>
+      <c r="E86">
+        <v>-29</v>
+      </c>
+      <c r="G86">
+        <v>92.5</v>
+      </c>
+      <c r="H86">
+        <v>6.8</v>
+      </c>
+      <c r="I86">
+        <v>83.1</v>
+      </c>
+      <c r="J86">
+        <v>-0.2</v>
+      </c>
+      <c r="K86">
+        <v>90.7</v>
+      </c>
+      <c r="L86">
         <v>7.7</v>
       </c>
-      <c r="E86">
-        <v>92.5</v>
-      </c>
-      <c r="F86">
-        <v>83.1</v>
-      </c>
-      <c r="G86">
-        <v>90.7</v>
-      </c>
-      <c r="H86">
+      <c r="N86">
         <v>88.6</v>
-      </c>
-      <c r="I86">
-        <v>854</v>
-      </c>
-      <c r="J86">
-        <v>-29</v>
-      </c>
-      <c r="L86">
-        <v>6.8</v>
-      </c>
-      <c r="M86">
-        <v>-0.2</v>
       </c>
       <c r="P86">
         <v>861</v>
@@ -42980,31 +42989,31 @@
         <v>37</v>
       </c>
       <c r="D87">
+        <v>715</v>
+      </c>
+      <c r="E87">
+        <v>-14</v>
+      </c>
+      <c r="G87">
+        <v>82.6</v>
+      </c>
+      <c r="H87">
+        <v>6.3</v>
+      </c>
+      <c r="I87">
+        <v>85.3</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="K87">
+        <v>90.7</v>
+      </c>
+      <c r="L87">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E87">
-        <v>82.6</v>
-      </c>
-      <c r="F87">
-        <v>85.3</v>
-      </c>
-      <c r="G87">
-        <v>90.7</v>
-      </c>
-      <c r="H87">
+      <c r="N87">
         <v>79.599999999999994</v>
-      </c>
-      <c r="I87">
-        <v>715</v>
-      </c>
-      <c r="J87">
-        <v>-14</v>
-      </c>
-      <c r="L87">
-        <v>6.3</v>
-      </c>
-      <c r="M87">
-        <v>1</v>
       </c>
       <c r="P87">
         <v>718</v>
@@ -43042,31 +43051,31 @@
         <v>37</v>
       </c>
       <c r="D88">
+        <v>842</v>
+      </c>
+      <c r="E88">
+        <v>-14</v>
+      </c>
+      <c r="G88">
+        <v>98.6</v>
+      </c>
+      <c r="H88">
+        <v>5.7</v>
+      </c>
+      <c r="I88">
+        <v>87.2</v>
+      </c>
+      <c r="J88">
+        <v>0.6</v>
+      </c>
+      <c r="K88">
+        <v>91.5</v>
+      </c>
+      <c r="L88">
         <v>3.8</v>
       </c>
-      <c r="E88">
-        <v>98.6</v>
-      </c>
-      <c r="F88">
-        <v>87.2</v>
-      </c>
-      <c r="G88">
-        <v>91.5</v>
-      </c>
-      <c r="H88">
+      <c r="N88">
         <v>83.5</v>
-      </c>
-      <c r="I88">
-        <v>842</v>
-      </c>
-      <c r="J88">
-        <v>-14</v>
-      </c>
-      <c r="L88">
-        <v>5.7</v>
-      </c>
-      <c r="M88">
-        <v>0.6</v>
       </c>
       <c r="P88">
         <v>845</v>
@@ -43104,31 +43113,31 @@
         <v>37</v>
       </c>
       <c r="D89">
+        <v>778</v>
+      </c>
+      <c r="E89">
+        <v>-15</v>
+      </c>
+      <c r="G89">
+        <v>89.7</v>
+      </c>
+      <c r="H89">
+        <v>5.4</v>
+      </c>
+      <c r="I89">
+        <v>85.4</v>
+      </c>
+      <c r="J89">
+        <v>-1.7</v>
+      </c>
+      <c r="K89">
+        <v>88.3</v>
+      </c>
+      <c r="L89">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E89">
-        <v>89.7</v>
-      </c>
-      <c r="F89">
-        <v>85.4</v>
-      </c>
-      <c r="G89">
-        <v>88.3</v>
-      </c>
-      <c r="H89">
+      <c r="N89">
         <v>82.3</v>
-      </c>
-      <c r="I89">
-        <v>778</v>
-      </c>
-      <c r="J89">
-        <v>-15</v>
-      </c>
-      <c r="L89">
-        <v>5.4</v>
-      </c>
-      <c r="M89">
-        <v>-1.7</v>
       </c>
       <c r="P89">
         <v>782</v>
@@ -43166,31 +43175,31 @@
         <v>37</v>
       </c>
       <c r="D90">
+        <v>808</v>
+      </c>
+      <c r="E90">
+        <v>-12</v>
+      </c>
+      <c r="G90">
+        <v>96</v>
+      </c>
+      <c r="H90">
+        <v>5.8</v>
+      </c>
+      <c r="I90">
+        <v>84.9</v>
+      </c>
+      <c r="J90">
+        <v>1.3</v>
+      </c>
+      <c r="K90">
+        <v>89.5</v>
+      </c>
+      <c r="L90">
         <v>3.3</v>
       </c>
-      <c r="E90">
-        <v>96</v>
-      </c>
-      <c r="F90">
-        <v>84.9</v>
-      </c>
-      <c r="G90">
-        <v>89.5</v>
-      </c>
-      <c r="H90">
+      <c r="N90">
         <v>84.2</v>
-      </c>
-      <c r="I90">
-        <v>808</v>
-      </c>
-      <c r="J90">
-        <v>-12</v>
-      </c>
-      <c r="L90">
-        <v>5.8</v>
-      </c>
-      <c r="M90">
-        <v>1.3</v>
       </c>
       <c r="P90">
         <v>810</v>
@@ -43228,31 +43237,31 @@
         <v>37</v>
       </c>
       <c r="D91">
+        <v>913</v>
+      </c>
+      <c r="E91">
+        <v>-15</v>
+      </c>
+      <c r="G91">
+        <v>76.7</v>
+      </c>
+      <c r="H91">
+        <v>3.5</v>
+      </c>
+      <c r="I91">
+        <v>85.8</v>
+      </c>
+      <c r="J91">
+        <v>-0.6</v>
+      </c>
+      <c r="K91">
+        <v>89.2</v>
+      </c>
+      <c r="L91">
         <v>3.9</v>
       </c>
-      <c r="E91">
-        <v>76.7</v>
-      </c>
-      <c r="F91">
-        <v>85.8</v>
-      </c>
-      <c r="G91">
-        <v>89.2</v>
-      </c>
-      <c r="H91">
+      <c r="N91">
         <v>81.7</v>
-      </c>
-      <c r="I91">
-        <v>913</v>
-      </c>
-      <c r="J91">
-        <v>-15</v>
-      </c>
-      <c r="L91">
-        <v>3.5</v>
-      </c>
-      <c r="M91">
-        <v>-0.6</v>
       </c>
       <c r="P91">
         <v>915</v>
@@ -43290,31 +43299,31 @@
         <v>37</v>
       </c>
       <c r="D92">
+        <v>784</v>
+      </c>
+      <c r="E92">
+        <v>-12</v>
+      </c>
+      <c r="G92">
+        <v>86</v>
+      </c>
+      <c r="H92">
+        <v>5.7</v>
+      </c>
+      <c r="I92">
+        <v>85.2</v>
+      </c>
+      <c r="J92">
+        <v>-0.2</v>
+      </c>
+      <c r="K92">
+        <v>88.6</v>
+      </c>
+      <c r="L92">
         <v>3.6</v>
       </c>
-      <c r="E92">
-        <v>86</v>
-      </c>
-      <c r="F92">
-        <v>85.2</v>
-      </c>
-      <c r="G92">
-        <v>88.6</v>
-      </c>
-      <c r="H92">
+      <c r="N92">
         <v>85.7</v>
-      </c>
-      <c r="I92">
-        <v>784</v>
-      </c>
-      <c r="J92">
-        <v>-12</v>
-      </c>
-      <c r="L92">
-        <v>5.7</v>
-      </c>
-      <c r="M92">
-        <v>-0.2</v>
       </c>
       <c r="P92">
         <v>786</v>
@@ -43352,31 +43361,31 @@
         <v>37</v>
       </c>
       <c r="D93">
+        <v>876</v>
+      </c>
+      <c r="E93">
+        <v>-11</v>
+      </c>
+      <c r="G93">
+        <v>93.1</v>
+      </c>
+      <c r="H93">
+        <v>6.8</v>
+      </c>
+      <c r="I93">
+        <v>85.6</v>
+      </c>
+      <c r="J93">
+        <v>1.7</v>
+      </c>
+      <c r="K93">
+        <v>90.3</v>
+      </c>
+      <c r="L93">
         <v>3</v>
       </c>
-      <c r="E93">
-        <v>93.1</v>
-      </c>
-      <c r="F93">
-        <v>85.6</v>
-      </c>
-      <c r="G93">
-        <v>90.3</v>
-      </c>
-      <c r="H93">
+      <c r="N93">
         <v>85.3</v>
-      </c>
-      <c r="I93">
-        <v>876</v>
-      </c>
-      <c r="J93">
-        <v>-11</v>
-      </c>
-      <c r="L93">
-        <v>6.8</v>
-      </c>
-      <c r="M93">
-        <v>1.7</v>
       </c>
       <c r="P93">
         <v>878</v>
@@ -43414,31 +43423,31 @@
         <v>37</v>
       </c>
       <c r="D94">
+        <v>811</v>
+      </c>
+      <c r="E94">
+        <v>-19</v>
+      </c>
+      <c r="G94">
+        <v>94.5</v>
+      </c>
+      <c r="H94">
+        <v>7.2</v>
+      </c>
+      <c r="I94">
+        <v>85.9</v>
+      </c>
+      <c r="J94">
+        <v>-2.7</v>
+      </c>
+      <c r="K94">
+        <v>88.6</v>
+      </c>
+      <c r="L94">
         <v>5.4</v>
       </c>
-      <c r="E94">
-        <v>94.5</v>
-      </c>
-      <c r="F94">
-        <v>85.9</v>
-      </c>
-      <c r="G94">
-        <v>88.6</v>
-      </c>
-      <c r="H94">
+      <c r="N94">
         <v>81.099999999999994</v>
-      </c>
-      <c r="I94">
-        <v>811</v>
-      </c>
-      <c r="J94">
-        <v>-19</v>
-      </c>
-      <c r="L94">
-        <v>7.2</v>
-      </c>
-      <c r="M94">
-        <v>-2.7</v>
       </c>
       <c r="P94">
         <v>815</v>
@@ -43476,31 +43485,31 @@
         <v>37</v>
       </c>
       <c r="D95">
+        <v>735</v>
+      </c>
+      <c r="E95">
+        <v>-11</v>
+      </c>
+      <c r="G95">
+        <v>78.3</v>
+      </c>
+      <c r="H95">
+        <v>6.1</v>
+      </c>
+      <c r="I95">
+        <v>85</v>
+      </c>
+      <c r="J95">
+        <v>0.2</v>
+      </c>
+      <c r="K95">
+        <v>88.8</v>
+      </c>
+      <c r="L95">
         <v>3.6</v>
       </c>
-      <c r="E95">
-        <v>78.3</v>
-      </c>
-      <c r="F95">
-        <v>85</v>
-      </c>
-      <c r="G95">
-        <v>88.8</v>
-      </c>
-      <c r="H95">
+      <c r="N95">
         <v>83.1</v>
-      </c>
-      <c r="I95">
-        <v>735</v>
-      </c>
-      <c r="J95">
-        <v>-11</v>
-      </c>
-      <c r="L95">
-        <v>6.1</v>
-      </c>
-      <c r="M95">
-        <v>0.2</v>
       </c>
       <c r="P95">
         <v>737</v>
@@ -43538,31 +43547,32 @@
         <v>37</v>
       </c>
       <c r="D96" s="10">
+        <v>885</v>
+      </c>
+      <c r="E96" s="10">
+        <v>-7</v>
+      </c>
+      <c r="G96" s="10">
+        <v>98.3</v>
+      </c>
+      <c r="H96" s="10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I96" s="10">
+        <v>84.2</v>
+      </c>
+      <c r="J96" s="10">
+        <v>3</v>
+      </c>
+      <c r="K96" s="10">
+        <v>89.2</v>
+      </c>
+      <c r="L96" s="10">
         <v>1.9</v>
       </c>
-      <c r="E96" s="10">
-        <v>98.3</v>
-      </c>
-      <c r="F96" s="10">
-        <v>84.2</v>
-      </c>
-      <c r="G96" s="10">
-        <v>89.2</v>
-      </c>
-      <c r="H96" s="10">
+      <c r="M96"/>
+      <c r="N96" s="10">
         <v>86.4</v>
-      </c>
-      <c r="I96" s="10">
-        <v>885</v>
-      </c>
-      <c r="J96" s="10">
-        <v>-7</v>
-      </c>
-      <c r="L96" s="10">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="M96" s="10">
-        <v>3</v>
       </c>
       <c r="P96" s="10">
         <v>836</v>
@@ -43600,31 +43610,31 @@
         <v>37</v>
       </c>
       <c r="D97">
+        <v>747</v>
+      </c>
+      <c r="E97">
+        <v>-31</v>
+      </c>
+      <c r="G97">
+        <v>92.8</v>
+      </c>
+      <c r="H97">
+        <v>7.2</v>
+      </c>
+      <c r="I97">
+        <v>81.3</v>
+      </c>
+      <c r="J97">
+        <v>1.5</v>
+      </c>
+      <c r="K97">
+        <v>92.2</v>
+      </c>
+      <c r="L97">
         <v>9.4</v>
       </c>
-      <c r="E97">
-        <v>92.8</v>
-      </c>
-      <c r="F97">
-        <v>81.3</v>
-      </c>
-      <c r="G97">
-        <v>92.2</v>
-      </c>
-      <c r="H97">
+      <c r="N97">
         <v>85.3</v>
-      </c>
-      <c r="I97">
-        <v>747</v>
-      </c>
-      <c r="J97">
-        <v>-31</v>
-      </c>
-      <c r="L97">
-        <v>7.2</v>
-      </c>
-      <c r="M97">
-        <v>1.5</v>
       </c>
       <c r="P97">
         <v>755</v>
@@ -43670,31 +43680,31 @@
         <v>37</v>
       </c>
       <c r="D99">
+        <v>746</v>
+      </c>
+      <c r="E99">
+        <v>-8</v>
+      </c>
+      <c r="G99">
+        <v>90.3</v>
+      </c>
+      <c r="H99">
+        <v>5.8</v>
+      </c>
+      <c r="I99">
+        <v>86.6</v>
+      </c>
+      <c r="J99">
+        <v>0.2</v>
+      </c>
+      <c r="K99">
+        <v>89.4</v>
+      </c>
+      <c r="L99">
         <v>2.6</v>
       </c>
-      <c r="E99">
-        <v>90.3</v>
-      </c>
-      <c r="F99">
-        <v>86.6</v>
-      </c>
-      <c r="G99">
-        <v>89.4</v>
-      </c>
-      <c r="H99">
+      <c r="N99">
         <v>86.1</v>
-      </c>
-      <c r="I99">
-        <v>746</v>
-      </c>
-      <c r="J99">
-        <v>-8</v>
-      </c>
-      <c r="L99">
-        <v>5.8</v>
-      </c>
-      <c r="M99">
-        <v>0.2</v>
       </c>
       <c r="P99">
         <v>747</v>
@@ -43732,31 +43742,31 @@
         <v>37</v>
       </c>
       <c r="D100">
+        <v>772</v>
+      </c>
+      <c r="E100">
+        <v>-13</v>
+      </c>
+      <c r="G100">
+        <v>94.4</v>
+      </c>
+      <c r="H100">
+        <v>6.3</v>
+      </c>
+      <c r="I100">
+        <v>85.2</v>
+      </c>
+      <c r="J100">
+        <v>-0.7</v>
+      </c>
+      <c r="K100">
+        <v>88.3</v>
+      </c>
+      <c r="L100">
         <v>3.8</v>
       </c>
-      <c r="E100">
-        <v>94.4</v>
-      </c>
-      <c r="F100">
-        <v>85.2</v>
-      </c>
-      <c r="G100">
-        <v>88.3</v>
-      </c>
-      <c r="H100">
+      <c r="N100">
         <v>82.2</v>
-      </c>
-      <c r="I100">
-        <v>772</v>
-      </c>
-      <c r="J100">
-        <v>-13</v>
-      </c>
-      <c r="L100">
-        <v>6.3</v>
-      </c>
-      <c r="M100">
-        <v>-0.7</v>
       </c>
       <c r="P100">
         <v>775</v>
@@ -43794,31 +43804,31 @@
         <v>37</v>
       </c>
       <c r="D101">
+        <v>812</v>
+      </c>
+      <c r="E101">
+        <v>-11</v>
+      </c>
+      <c r="G101">
+        <v>87.6</v>
+      </c>
+      <c r="H101">
+        <v>5.8</v>
+      </c>
+      <c r="I101">
+        <v>85.4</v>
+      </c>
+      <c r="J101">
+        <v>0.1</v>
+      </c>
+      <c r="K101">
+        <v>88.5</v>
+      </c>
+      <c r="L101">
         <v>3</v>
       </c>
-      <c r="E101">
-        <v>87.6</v>
-      </c>
-      <c r="F101">
-        <v>85.4</v>
-      </c>
-      <c r="G101">
-        <v>88.5</v>
-      </c>
-      <c r="H101">
+      <c r="N101">
         <v>82</v>
-      </c>
-      <c r="I101">
-        <v>812</v>
-      </c>
-      <c r="J101">
-        <v>-11</v>
-      </c>
-      <c r="L101">
-        <v>5.8</v>
-      </c>
-      <c r="M101">
-        <v>0.1</v>
       </c>
       <c r="P101">
         <v>814</v>
@@ -43856,31 +43866,31 @@
         <v>37</v>
       </c>
       <c r="D102">
+        <v>694</v>
+      </c>
+      <c r="E102">
+        <v>-20</v>
+      </c>
+      <c r="G102">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="H102">
+        <v>5.6</v>
+      </c>
+      <c r="I102">
+        <v>82.2</v>
+      </c>
+      <c r="J102">
+        <v>-1.5</v>
+      </c>
+      <c r="K102">
+        <v>87.3</v>
+      </c>
+      <c r="L102">
         <v>6.6</v>
       </c>
-      <c r="E102">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="F102">
-        <v>82.2</v>
-      </c>
-      <c r="G102">
-        <v>87.3</v>
-      </c>
-      <c r="H102">
+      <c r="N102">
         <v>83.6</v>
-      </c>
-      <c r="I102">
-        <v>694</v>
-      </c>
-      <c r="J102">
-        <v>-20</v>
-      </c>
-      <c r="L102">
-        <v>5.6</v>
-      </c>
-      <c r="M102">
-        <v>-1.5</v>
       </c>
       <c r="P102">
         <v>699</v>
@@ -43918,31 +43928,32 @@
         <v>37</v>
       </c>
       <c r="D103" s="10">
+        <v>805</v>
+      </c>
+      <c r="E103" s="10">
+        <v>-6</v>
+      </c>
+      <c r="G103" s="10">
+        <v>85.1</v>
+      </c>
+      <c r="H103" s="10">
+        <v>5.8</v>
+      </c>
+      <c r="I103" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="J103" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="K103" s="10">
+        <v>88</v>
+      </c>
+      <c r="L103" s="10">
         <v>1.7</v>
       </c>
-      <c r="E103" s="10">
-        <v>85.1</v>
-      </c>
-      <c r="F103" s="10">
-        <v>86.1</v>
-      </c>
-      <c r="G103" s="10">
-        <v>88</v>
-      </c>
-      <c r="H103" s="10">
+      <c r="M103"/>
+      <c r="N103" s="10">
         <v>78.8</v>
-      </c>
-      <c r="I103" s="10">
-        <v>805</v>
-      </c>
-      <c r="J103" s="10">
-        <v>-6</v>
-      </c>
-      <c r="L103" s="10">
-        <v>5.8</v>
-      </c>
-      <c r="M103" s="10">
-        <v>0.2</v>
       </c>
       <c r="P103" s="10">
         <v>805</v>
@@ -43980,31 +43991,31 @@
         <v>37</v>
       </c>
       <c r="D104">
+        <v>822</v>
+      </c>
+      <c r="E104">
+        <v>-10</v>
+      </c>
+      <c r="G104">
+        <v>84.1</v>
+      </c>
+      <c r="H104">
+        <v>6.6</v>
+      </c>
+      <c r="I104">
+        <v>84.9</v>
+      </c>
+      <c r="J104">
+        <v>1.3</v>
+      </c>
+      <c r="K104">
+        <v>86.2</v>
+      </c>
+      <c r="L104">
         <v>2.7</v>
       </c>
-      <c r="E104">
-        <v>84.1</v>
-      </c>
-      <c r="F104">
-        <v>84.9</v>
-      </c>
-      <c r="G104">
-        <v>86.2</v>
-      </c>
-      <c r="H104">
+      <c r="N104">
         <v>81.5</v>
-      </c>
-      <c r="I104">
-        <v>822</v>
-      </c>
-      <c r="J104">
-        <v>-10</v>
-      </c>
-      <c r="L104">
-        <v>6.6</v>
-      </c>
-      <c r="M104">
-        <v>1.3</v>
       </c>
       <c r="P104">
         <v>810</v>
@@ -44042,31 +44053,32 @@
         <v>37</v>
       </c>
       <c r="D105" s="10">
+        <v>842</v>
+      </c>
+      <c r="E105" s="10">
+        <v>-7</v>
+      </c>
+      <c r="G105" s="10">
+        <v>93.3</v>
+      </c>
+      <c r="H105" s="10">
+        <v>5.9</v>
+      </c>
+      <c r="I105" s="10">
+        <v>88.5</v>
+      </c>
+      <c r="J105" s="10">
+        <v>-2.5</v>
+      </c>
+      <c r="K105" s="10">
+        <v>87.9</v>
+      </c>
+      <c r="L105" s="10">
         <v>1.9</v>
       </c>
-      <c r="E105" s="10">
-        <v>93.3</v>
-      </c>
-      <c r="F105" s="10">
-        <v>88.5</v>
-      </c>
-      <c r="G105" s="10">
-        <v>87.9</v>
-      </c>
-      <c r="H105" s="10">
+      <c r="M105"/>
+      <c r="N105" s="10">
         <v>76.5</v>
-      </c>
-      <c r="I105" s="10">
-        <v>842</v>
-      </c>
-      <c r="J105" s="10">
-        <v>-7</v>
-      </c>
-      <c r="L105" s="10">
-        <v>5.9</v>
-      </c>
-      <c r="M105" s="10">
-        <v>-2.5</v>
       </c>
       <c r="P105" s="10">
         <v>843</v>
@@ -44104,31 +44116,32 @@
         <v>37</v>
       </c>
       <c r="D106" s="10">
+        <v>826</v>
+      </c>
+      <c r="E106" s="10">
+        <v>-9</v>
+      </c>
+      <c r="G106" s="10">
+        <v>86.3</v>
+      </c>
+      <c r="H106" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="I106" s="10">
+        <v>86.7</v>
+      </c>
+      <c r="J106" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="K106" s="10">
+        <v>91.1</v>
+      </c>
+      <c r="L106" s="10">
         <v>2.6</v>
       </c>
-      <c r="E106" s="10">
-        <v>86.3</v>
-      </c>
-      <c r="F106" s="10">
-        <v>86.7</v>
-      </c>
-      <c r="G106" s="10">
-        <v>91.1</v>
-      </c>
-      <c r="H106" s="10">
+      <c r="M106"/>
+      <c r="N106" s="10">
         <v>89</v>
-      </c>
-      <c r="I106" s="10">
-        <v>826</v>
-      </c>
-      <c r="J106" s="10">
-        <v>-9</v>
-      </c>
-      <c r="L106" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="M106" s="10">
-        <v>1.8</v>
       </c>
       <c r="P106" s="10">
         <v>828</v>
@@ -44166,31 +44179,31 @@
         <v>37</v>
       </c>
       <c r="D107">
+        <v>921</v>
+      </c>
+      <c r="E107">
+        <v>-15</v>
+      </c>
+      <c r="G107">
+        <v>95.6</v>
+      </c>
+      <c r="H107">
+        <v>9.1</v>
+      </c>
+      <c r="I107">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="J107">
+        <v>3</v>
+      </c>
+      <c r="K107">
+        <v>87.1</v>
+      </c>
+      <c r="L107">
         <v>3.7</v>
       </c>
-      <c r="E107">
-        <v>95.6</v>
-      </c>
-      <c r="F107">
-        <v>80.400000000000006</v>
-      </c>
-      <c r="G107">
-        <v>87.1</v>
-      </c>
-      <c r="H107">
+      <c r="N107">
         <v>86.8</v>
-      </c>
-      <c r="I107">
-        <v>921</v>
-      </c>
-      <c r="J107">
-        <v>-15</v>
-      </c>
-      <c r="L107">
-        <v>9.1</v>
-      </c>
-      <c r="M107">
-        <v>3</v>
       </c>
       <c r="P107">
         <v>924</v>
@@ -44228,31 +44241,31 @@
         <v>37</v>
       </c>
       <c r="D108">
+        <v>842</v>
+      </c>
+      <c r="E108">
+        <v>-12</v>
+      </c>
+      <c r="G108">
+        <v>95.7</v>
+      </c>
+      <c r="H108">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I108">
+        <v>86.4</v>
+      </c>
+      <c r="J108">
+        <v>0.9</v>
+      </c>
+      <c r="K108">
+        <v>90.6</v>
+      </c>
+      <c r="L108">
         <v>3.4</v>
       </c>
-      <c r="E108">
-        <v>95.7</v>
-      </c>
-      <c r="F108">
-        <v>86.4</v>
-      </c>
-      <c r="G108">
-        <v>90.6</v>
-      </c>
-      <c r="H108">
+      <c r="N108">
         <v>86.1</v>
-      </c>
-      <c r="I108">
-        <v>842</v>
-      </c>
-      <c r="J108">
-        <v>-12</v>
-      </c>
-      <c r="L108">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="M108">
-        <v>0.9</v>
       </c>
       <c r="P108">
         <v>844</v>
@@ -44290,31 +44303,31 @@
         <v>37</v>
       </c>
       <c r="D109">
+        <v>874</v>
+      </c>
+      <c r="E109">
+        <v>-12</v>
+      </c>
+      <c r="G109">
+        <v>86.5</v>
+      </c>
+      <c r="H109">
+        <v>6</v>
+      </c>
+      <c r="I109">
+        <v>85.6</v>
+      </c>
+      <c r="J109">
+        <v>1.2</v>
+      </c>
+      <c r="K109">
+        <v>89.9</v>
+      </c>
+      <c r="L109">
         <v>3.1</v>
       </c>
-      <c r="E109">
-        <v>86.5</v>
-      </c>
-      <c r="F109">
-        <v>85.6</v>
-      </c>
-      <c r="G109">
-        <v>89.9</v>
-      </c>
-      <c r="H109">
+      <c r="N109">
         <v>84.7</v>
-      </c>
-      <c r="I109">
-        <v>874</v>
-      </c>
-      <c r="J109">
-        <v>-12</v>
-      </c>
-      <c r="L109">
-        <v>6</v>
-      </c>
-      <c r="M109">
-        <v>1.2</v>
       </c>
       <c r="P109">
         <v>876</v>
@@ -44360,31 +44373,31 @@
         <v>37</v>
       </c>
       <c r="D111">
+        <v>791</v>
+      </c>
+      <c r="E111">
+        <v>-17</v>
+      </c>
+      <c r="G111">
+        <v>83.5</v>
+      </c>
+      <c r="H111">
+        <v>6.9</v>
+      </c>
+      <c r="I111">
+        <v>83.2</v>
+      </c>
+      <c r="J111">
+        <v>0.9</v>
+      </c>
+      <c r="K111">
+        <v>89.1</v>
+      </c>
+      <c r="L111">
         <v>5</v>
       </c>
-      <c r="E111">
-        <v>83.5</v>
-      </c>
-      <c r="F111">
-        <v>83.2</v>
-      </c>
-      <c r="G111">
-        <v>89.1</v>
-      </c>
-      <c r="H111">
+      <c r="N111">
         <v>83.9</v>
-      </c>
-      <c r="I111">
-        <v>791</v>
-      </c>
-      <c r="J111">
-        <v>-17</v>
-      </c>
-      <c r="L111">
-        <v>6.9</v>
-      </c>
-      <c r="M111">
-        <v>0.9</v>
       </c>
       <c r="P111">
         <v>794</v>
@@ -44422,31 +44435,31 @@
         <v>37</v>
       </c>
       <c r="D112">
+        <v>821</v>
+      </c>
+      <c r="E112">
+        <v>-19</v>
+      </c>
+      <c r="G112">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="H112">
+        <v>6</v>
+      </c>
+      <c r="I112">
+        <v>86.8</v>
+      </c>
+      <c r="J112">
+        <v>-2.1</v>
+      </c>
+      <c r="K112">
+        <v>90</v>
+      </c>
+      <c r="L112">
         <v>5.3</v>
       </c>
-      <c r="E112">
-        <v>76.900000000000006</v>
-      </c>
-      <c r="F112">
-        <v>86.8</v>
-      </c>
-      <c r="G112">
-        <v>90</v>
-      </c>
-      <c r="H112">
+      <c r="N112">
         <v>94.6</v>
-      </c>
-      <c r="I112">
-        <v>821</v>
-      </c>
-      <c r="J112">
-        <v>-19</v>
-      </c>
-      <c r="L112">
-        <v>6</v>
-      </c>
-      <c r="M112">
-        <v>-2.1</v>
       </c>
       <c r="P112">
         <v>824</v>
@@ -44484,31 +44497,31 @@
         <v>37</v>
       </c>
       <c r="D113">
+        <v>891</v>
+      </c>
+      <c r="E113">
+        <v>-14</v>
+      </c>
+      <c r="G113">
+        <v>89.3</v>
+      </c>
+      <c r="H113">
+        <v>5.9</v>
+      </c>
+      <c r="I113">
+        <v>85.4</v>
+      </c>
+      <c r="J113">
+        <v>0.9</v>
+      </c>
+      <c r="K113">
+        <v>89.8</v>
+      </c>
+      <c r="L113">
         <v>3.6</v>
       </c>
-      <c r="E113">
-        <v>89.3</v>
-      </c>
-      <c r="F113">
-        <v>85.4</v>
-      </c>
-      <c r="G113">
-        <v>89.8</v>
-      </c>
-      <c r="H113">
+      <c r="N113">
         <v>86.9</v>
-      </c>
-      <c r="I113">
-        <v>891</v>
-      </c>
-      <c r="J113">
-        <v>-14</v>
-      </c>
-      <c r="L113">
-        <v>5.9</v>
-      </c>
-      <c r="M113">
-        <v>0.9</v>
       </c>
       <c r="P113">
         <v>893</v>
@@ -44546,31 +44559,32 @@
         <v>37</v>
       </c>
       <c r="D114" s="10">
+        <v>875</v>
+      </c>
+      <c r="E114" s="10">
+        <v>-9</v>
+      </c>
+      <c r="G114" s="10">
+        <v>82.7</v>
+      </c>
+      <c r="H114" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="I114" s="10">
+        <v>85.8</v>
+      </c>
+      <c r="J114" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="K114" s="10">
+        <v>89</v>
+      </c>
+      <c r="L114" s="10">
         <v>2.4</v>
       </c>
-      <c r="E114" s="10">
-        <v>82.7</v>
-      </c>
-      <c r="F114" s="10">
-        <v>85.8</v>
-      </c>
-      <c r="G114" s="10">
-        <v>89</v>
-      </c>
-      <c r="H114" s="10">
+      <c r="M114"/>
+      <c r="N114" s="10">
         <v>85.9</v>
-      </c>
-      <c r="I114" s="10">
-        <v>875</v>
-      </c>
-      <c r="J114" s="10">
-        <v>-9</v>
-      </c>
-      <c r="L114" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="M114" s="10">
-        <v>0.8</v>
       </c>
       <c r="P114" s="10">
         <v>877</v>
@@ -44608,31 +44622,31 @@
         <v>37</v>
       </c>
       <c r="D115">
+        <v>828</v>
+      </c>
+      <c r="E115">
+        <v>-19</v>
+      </c>
+      <c r="G115">
+        <v>85.3</v>
+      </c>
+      <c r="H115">
+        <v>6.5</v>
+      </c>
+      <c r="I115">
+        <v>85.4</v>
+      </c>
+      <c r="J115">
+        <v>-0.3</v>
+      </c>
+      <c r="K115">
+        <v>90.3</v>
+      </c>
+      <c r="L115">
         <v>5.3</v>
       </c>
-      <c r="E115">
-        <v>85.3</v>
-      </c>
-      <c r="F115">
-        <v>85.4</v>
-      </c>
-      <c r="G115">
-        <v>90.3</v>
-      </c>
-      <c r="H115">
+      <c r="N115">
         <v>84.7</v>
-      </c>
-      <c r="I115">
-        <v>828</v>
-      </c>
-      <c r="J115">
-        <v>-19</v>
-      </c>
-      <c r="L115">
-        <v>6.5</v>
-      </c>
-      <c r="M115">
-        <v>-0.3</v>
       </c>
       <c r="P115">
         <v>831</v>
@@ -44670,31 +44684,31 @@
         <v>37</v>
       </c>
       <c r="D116">
+        <v>948</v>
+      </c>
+      <c r="E116">
+        <v>-36</v>
+      </c>
+      <c r="G116">
+        <v>90</v>
+      </c>
+      <c r="H116">
+        <v>5.8</v>
+      </c>
+      <c r="I116">
+        <v>80</v>
+      </c>
+      <c r="J116">
+        <v>1.2</v>
+      </c>
+      <c r="K116">
+        <v>89.9</v>
+      </c>
+      <c r="L116">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E116">
-        <v>90</v>
-      </c>
-      <c r="F116">
-        <v>80</v>
-      </c>
-      <c r="G116">
-        <v>89.9</v>
-      </c>
-      <c r="H116">
+      <c r="N116">
         <v>85.8</v>
-      </c>
-      <c r="I116">
-        <v>948</v>
-      </c>
-      <c r="J116">
-        <v>-36</v>
-      </c>
-      <c r="L116">
-        <v>5.8</v>
-      </c>
-      <c r="M116">
-        <v>1.2</v>
       </c>
       <c r="P116">
         <v>956</v>
@@ -44732,31 +44746,31 @@
         <v>37</v>
       </c>
       <c r="D117">
+        <v>744</v>
+      </c>
+      <c r="E117">
+        <v>-24</v>
+      </c>
+      <c r="G117">
+        <v>90.7</v>
+      </c>
+      <c r="H117">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I117">
+        <v>85.5</v>
+      </c>
+      <c r="J117">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="K117">
+        <v>91.9</v>
+      </c>
+      <c r="L117">
         <v>7.5</v>
       </c>
-      <c r="E117">
-        <v>90.7</v>
-      </c>
-      <c r="F117">
-        <v>85.5</v>
-      </c>
-      <c r="G117">
-        <v>91.9</v>
-      </c>
-      <c r="H117">
+      <c r="N117">
         <v>85.8</v>
-      </c>
-      <c r="I117">
-        <v>744</v>
-      </c>
-      <c r="J117">
-        <v>-24</v>
-      </c>
-      <c r="L117">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M117">
-        <v>-1.1000000000000001</v>
       </c>
       <c r="P117">
         <v>749</v>
@@ -44794,31 +44808,31 @@
         <v>37</v>
       </c>
       <c r="D118">
+        <v>865</v>
+      </c>
+      <c r="E118">
+        <v>-15</v>
+      </c>
+      <c r="G118">
+        <v>83.6</v>
+      </c>
+      <c r="H118">
+        <v>5.2</v>
+      </c>
+      <c r="I118">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="J118">
+        <v>1.7</v>
+      </c>
+      <c r="K118">
+        <v>86.8</v>
+      </c>
+      <c r="L118">
         <v>4</v>
       </c>
-      <c r="E118">
-        <v>83.6</v>
-      </c>
-      <c r="F118">
-        <v>81.099999999999994</v>
-      </c>
-      <c r="G118">
-        <v>86.8</v>
-      </c>
-      <c r="H118">
+      <c r="N118">
         <v>84</v>
-      </c>
-      <c r="I118">
-        <v>865</v>
-      </c>
-      <c r="J118">
-        <v>-15</v>
-      </c>
-      <c r="L118">
-        <v>5.2</v>
-      </c>
-      <c r="M118">
-        <v>1.7</v>
       </c>
       <c r="P118">
         <v>868</v>
@@ -44856,31 +44870,31 @@
         <v>37</v>
       </c>
       <c r="D119">
+        <v>793</v>
+      </c>
+      <c r="E119">
+        <v>-15</v>
+      </c>
+      <c r="G119">
+        <v>89.3</v>
+      </c>
+      <c r="H119">
+        <v>5.6</v>
+      </c>
+      <c r="I119">
+        <v>86</v>
+      </c>
+      <c r="J119">
+        <v>-0.4</v>
+      </c>
+      <c r="K119">
+        <v>90</v>
+      </c>
+      <c r="L119">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E119">
-        <v>89.3</v>
-      </c>
-      <c r="F119">
-        <v>86</v>
-      </c>
-      <c r="G119">
-        <v>90</v>
-      </c>
-      <c r="H119">
+      <c r="N119">
         <v>88.1</v>
-      </c>
-      <c r="I119">
-        <v>793</v>
-      </c>
-      <c r="J119">
-        <v>-15</v>
-      </c>
-      <c r="L119">
-        <v>5.6</v>
-      </c>
-      <c r="M119">
-        <v>-0.4</v>
       </c>
       <c r="P119">
         <v>783</v>
@@ -44923,6 +44937,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1659F713-B10A-438D-B10C-176BDBBB1D49}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CA8922-6348-7449-90AE-31A0CD7BA56C}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>